<commit_message>
Actualizaci├│n proveedores desde PC de Naty
</commit_message>
<xml_diff>
--- a/data/proveedores.xlsx
+++ b/data/proveedores.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="365">
   <si>
     <t>cui</t>
   </si>
@@ -664,9 +664,6 @@
     <t>nombre</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>20-14057613-2</t>
   </si>
   <si>
@@ -1045,7 +1042,82 @@
     <t>2063hqid</t>
   </si>
   <si>
-    <t>zz</t>
+    <t>clave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARCIA CARLOS   </t>
+  </si>
+  <si>
+    <t>20-14057622-1</t>
+  </si>
+  <si>
+    <t>2255gcsa</t>
+  </si>
+  <si>
+    <t>33-71593533-9</t>
+  </si>
+  <si>
+    <t>SAGA SRL</t>
+  </si>
+  <si>
+    <t>6988sgsu</t>
+  </si>
+  <si>
+    <t>PIPS S.A.S</t>
+  </si>
+  <si>
+    <t>30-71683127-9</t>
+  </si>
+  <si>
+    <t>3235poññ</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>PATAGONIA VIVA SRL</t>
+  </si>
+  <si>
+    <t>30-70813798-3</t>
+  </si>
+  <si>
+    <t>2001patv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIKRONK SRL </t>
+  </si>
+  <si>
+    <t>30-71518604-3</t>
+  </si>
+  <si>
+    <t>6214skrk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J.B. FILIPPI S.R.L </t>
+  </si>
+  <si>
+    <t>30-71474343-7</t>
+  </si>
+  <si>
+    <t>1415jbfp</t>
+  </si>
+  <si>
+    <t>RIVAS ORELLANA DIEGO ARIEL</t>
+  </si>
+  <si>
+    <t>20-29458029-9</t>
+  </si>
+  <si>
+    <t>5459rvdo</t>
+  </si>
+  <si>
+    <t>MUNGAI S.R.L</t>
+  </si>
+  <si>
+    <t>30-71728178-7</t>
+  </si>
+  <si>
+    <t>1418mngs</t>
   </si>
 </sst>
 </file>
@@ -1389,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>213</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1421,7 +1493,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1432,7 +1504,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1443,7 +1515,7 @@
         <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1454,7 +1526,7 @@
         <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,7 +1537,7 @@
         <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1476,7 +1548,7 @@
         <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1487,7 +1559,7 @@
         <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1498,7 +1570,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1509,7 +1581,7 @@
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1520,7 +1592,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,7 +1603,7 @@
         <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1542,7 +1614,7 @@
         <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1553,7 +1625,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1564,7 +1636,7 @@
         <v>201</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1575,7 +1647,7 @@
         <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1586,7 +1658,7 @@
         <v>114</v>
       </c>
       <c r="C17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1597,7 +1669,7 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1608,7 +1680,7 @@
         <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1619,7 +1691,7 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1630,7 +1702,7 @@
         <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1641,7 +1713,7 @@
         <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1652,7 +1724,7 @@
         <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,7 +1735,7 @@
         <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1674,7 +1746,7 @@
         <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1685,7 +1757,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1696,7 +1768,7 @@
         <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1707,7 +1779,7 @@
         <v>130</v>
       </c>
       <c r="C28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1718,7 +1790,7 @@
         <v>179</v>
       </c>
       <c r="C29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1729,7 +1801,7 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1740,7 +1812,7 @@
         <v>191</v>
       </c>
       <c r="C31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1751,7 +1823,7 @@
         <v>209</v>
       </c>
       <c r="C32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1762,7 +1834,7 @@
         <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1773,7 +1845,7 @@
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1784,7 +1856,7 @@
         <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1795,7 +1867,7 @@
         <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1806,7 +1878,7 @@
         <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1817,7 +1889,7 @@
         <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1828,7 +1900,7 @@
         <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1839,7 +1911,7 @@
         <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1850,7 +1922,7 @@
         <v>146</v>
       </c>
       <c r="C41" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1861,7 +1933,7 @@
         <v>167</v>
       </c>
       <c r="C42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1872,7 +1944,7 @@
         <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1883,7 +1955,7 @@
         <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1894,7 +1966,7 @@
         <v>144</v>
       </c>
       <c r="C45" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1905,7 +1977,7 @@
         <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1916,7 +1988,7 @@
         <v>154</v>
       </c>
       <c r="C47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1927,7 +1999,7 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1938,7 +2010,7 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1949,7 +2021,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1960,7 +2032,7 @@
         <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1971,7 +2043,7 @@
         <v>177</v>
       </c>
       <c r="C52" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1982,7 +2054,7 @@
         <v>148</v>
       </c>
       <c r="C53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1993,7 +2065,7 @@
         <v>199</v>
       </c>
       <c r="C54" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2004,7 +2076,7 @@
         <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2015,7 +2087,7 @@
         <v>126</v>
       </c>
       <c r="C56" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,7 +2098,7 @@
         <v>161</v>
       </c>
       <c r="C57" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2037,7 +2109,7 @@
         <v>171</v>
       </c>
       <c r="C58" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2048,7 +2120,7 @@
         <v>106</v>
       </c>
       <c r="C59" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2059,7 +2131,7 @@
         <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2070,7 +2142,7 @@
         <v>32</v>
       </c>
       <c r="C61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2081,7 +2153,7 @@
         <v>189</v>
       </c>
       <c r="C62" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2092,7 +2164,7 @@
         <v>138</v>
       </c>
       <c r="C63" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2103,7 +2175,7 @@
         <v>118</v>
       </c>
       <c r="C64" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2114,7 +2186,7 @@
         <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2125,7 +2197,7 @@
         <v>205</v>
       </c>
       <c r="C66" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2208,7 @@
         <v>181</v>
       </c>
       <c r="C67" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2147,7 +2219,7 @@
         <v>74</v>
       </c>
       <c r="C68" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,7 +2230,7 @@
         <v>64</v>
       </c>
       <c r="C69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2169,7 +2241,7 @@
         <v>134</v>
       </c>
       <c r="C70" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2180,7 +2252,7 @@
         <v>136</v>
       </c>
       <c r="C71" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2191,7 +2263,7 @@
         <v>157</v>
       </c>
       <c r="C72" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2202,7 +2274,7 @@
         <v>175</v>
       </c>
       <c r="C73" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,7 +2285,7 @@
         <v>150</v>
       </c>
       <c r="C74" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,7 +2296,7 @@
         <v>173</v>
       </c>
       <c r="C75" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2235,7 +2307,7 @@
         <v>34</v>
       </c>
       <c r="C76" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2246,7 +2318,7 @@
         <v>197</v>
       </c>
       <c r="C77" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2257,7 +2329,7 @@
         <v>38</v>
       </c>
       <c r="C78" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,7 +2340,7 @@
         <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2351,7 @@
         <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2362,7 @@
         <v>185</v>
       </c>
       <c r="C81" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2373,7 @@
         <v>42</v>
       </c>
       <c r="C82" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,7 +2384,7 @@
         <v>124</v>
       </c>
       <c r="C83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2395,7 @@
         <v>116</v>
       </c>
       <c r="C84" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2406,7 @@
         <v>203</v>
       </c>
       <c r="C85" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,18 +2417,18 @@
         <v>60</v>
       </c>
       <c r="C86" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B87" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C87" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2439,7 @@
         <v>44</v>
       </c>
       <c r="C88" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2378,7 +2450,7 @@
         <v>163</v>
       </c>
       <c r="C89" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2389,7 +2461,7 @@
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,7 +2472,7 @@
         <v>165</v>
       </c>
       <c r="C91" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2411,7 +2483,7 @@
         <v>40</v>
       </c>
       <c r="C92" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2422,7 +2494,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2433,7 +2505,7 @@
         <v>104</v>
       </c>
       <c r="C94" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2444,7 +2516,7 @@
         <v>193</v>
       </c>
       <c r="C95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2455,7 +2527,7 @@
         <v>140</v>
       </c>
       <c r="C96" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2466,7 +2538,7 @@
         <v>159</v>
       </c>
       <c r="C97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,7 +2549,7 @@
         <v>28</v>
       </c>
       <c r="C98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,7 +2560,7 @@
         <v>84</v>
       </c>
       <c r="C99" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2499,7 +2571,7 @@
         <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2510,7 +2582,7 @@
         <v>80</v>
       </c>
       <c r="C101" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2521,7 +2593,7 @@
         <v>68</v>
       </c>
       <c r="C102" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2532,7 +2604,7 @@
         <v>78</v>
       </c>
       <c r="C103" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -2543,7 +2615,7 @@
         <v>183</v>
       </c>
       <c r="C104" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2554,7 +2626,7 @@
         <v>72</v>
       </c>
       <c r="C105" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,7 +2637,7 @@
         <v>58</v>
       </c>
       <c r="C106" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2576,7 +2648,7 @@
         <v>195</v>
       </c>
       <c r="C107" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2587,73 +2659,161 @@
         <v>211</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>320</v>
+      </c>
+      <c r="B109" t="s">
         <v>321</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>323</v>
+      </c>
+      <c r="B110" t="s">
         <v>324</v>
       </c>
-      <c r="B110" t="s">
-        <v>325</v>
-      </c>
       <c r="C110" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>325</v>
+      </c>
+      <c r="B111" t="s">
         <v>326</v>
       </c>
-      <c r="B111" t="s">
-        <v>327</v>
-      </c>
       <c r="C111" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>327</v>
+      </c>
+      <c r="B112" t="s">
         <v>328</v>
       </c>
-      <c r="B112" t="s">
-        <v>329</v>
-      </c>
       <c r="C112" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>329</v>
+      </c>
+      <c r="B113" t="s">
         <v>330</v>
       </c>
-      <c r="B113" t="s">
-        <v>331</v>
-      </c>
       <c r="C113" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>335</v>
+      </c>
+      <c r="B114" t="s">
         <v>336</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C114" s="2" t="s">
-        <v>338</v>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>340</v>
+      </c>
+      <c r="B115" t="s">
+        <v>341</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>344</v>
+      </c>
+      <c r="B116" t="s">
+        <v>343</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>346</v>
+      </c>
+      <c r="B117" t="s">
+        <v>347</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>350</v>
+      </c>
+      <c r="B118" t="s">
+        <v>351</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>353</v>
+      </c>
+      <c r="B119" t="s">
+        <v>354</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>356</v>
+      </c>
+      <c r="B120" t="s">
+        <v>357</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>359</v>
+      </c>
+      <c r="B121" t="s">
+        <v>360</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>362</v>
+      </c>
+      <c r="B122" t="s">
+        <v>363</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>